<commit_message>
Fix FastAPI endpoints and upload page for Vercel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Project</t>
   </si>
@@ -60,10 +60,10 @@
     <t>Award</t>
   </si>
   <si>
-    <t>MANAGERS</t>
+    <t>staff</t>
   </si>
   <si>
-    <t>MABAGERS VALUES RM</t>
+    <t>staff VALUES RM</t>
   </si>
   <si>
     <t>Remark</t>
@@ -73,15 +73,6 @@
   </si>
   <si>
     <t xml:space="preserve">compeleted </t>
-  </si>
-  <si>
-    <t>CDS (Enter date DD/MM/YYYY)</t>
-  </si>
-  <si>
-    <t>finish date (Enter date DD/MM/YYYY)</t>
-  </si>
-  <si>
-    <t>actual finish  date (Enter date DD/MM/YYYY)</t>
   </si>
   <si>
     <t>Materials &amp; Quantities:</t>
@@ -151,6 +142,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -209,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -226,6 +221,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -449,6 +450,8 @@
     <col customWidth="1" min="9" max="9" width="25.38"/>
     <col customWidth="1" min="11" max="11" width="30.13"/>
     <col customWidth="1" min="14" max="14" width="22.75"/>
+    <col customWidth="1" min="16" max="16" width="15.75"/>
+    <col customWidth="1" min="17" max="17" width="18.63"/>
     <col customWidth="1" min="19" max="19" width="23.5"/>
   </cols>
   <sheetData>
@@ -522,12 +525,12 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="4" t="s">
-        <v>20</v>
+      <c r="I2" s="6">
+        <v>45658.0</v>
       </c>
       <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
+      <c r="K2" s="7">
+        <v>45690.0</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -536,8 +539,8 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
-      <c r="S2" s="4" t="s">
-        <v>22</v>
+      <c r="S2" s="6">
+        <v>45719.0</v>
       </c>
     </row>
     <row r="3">
@@ -21503,17 +21506,8 @@
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="N2:N1000">
       <formula1>IF(N2="", 0, N2)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="I2:I1000 K2:K1000">
-      <formula1>AND(ISDATE(I3), I2&lt;&gt;"")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="R2:R1000">
-      <formula1>AND(ISTEXT(R2), R2&lt;&gt;"")</formula1>
-    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="F2:G1000">
       <formula1>AND(ISNUMBER(F2), F2&lt;&gt;"")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="L2:L1000">
-      <formula1>AND(L2&lt;&gt;"", COUNTIF(Sheet2!A:A, L2))</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="E2:E1000">
       <formula1>AND(ISNUMBER(E2), E2&gt;=0, E2&lt;=100, E2&lt;&gt;"")</formula1>
@@ -21521,20 +21515,32 @@
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="A2:C1000">
       <formula1>AND(ISTEXT(A1), A1&lt;&gt;"")</formula1>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="M2:M1000">
+      <formula1>AND(ISNUMBER(M2), M2&gt;=0, M2&lt;&gt;"")</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="O2:P1000">
+      <formula1>AND(ISTEXT(O2), O2&lt;&gt;" ")</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="I1:I1000">
+      <formula1>AND(ISDATE(I1), NOT(ISBLANK(I1)))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="S1:S1000">
+      <formula1>AND(ISDATE(S1), NOT(ISBLANK(S1)), S1&gt;I1)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="R2:R1000">
+      <formula1>AND(ISTEXT(R2), R2&lt;&gt;"")</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="L2:L1000">
+      <formula1>AND(L2&lt;&gt;"", COUNTIF(Sheet2!A:A, L2))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="K1:K1000">
+      <formula1>AND(ISDATE(K1), NOT(ISBLANK(K1)), K1&gt;I1)</formula1>
+    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="H2:H1000 J2:J1000 Q2:Q1000">
       <formula1>AND(ISNUMBER(H2), H2&gt;=0, H2&lt;&gt;" ")</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D1000">
       <formula1>"ongoing ,compeleted ,hold ,postpond "</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="S2:S1000">
-      <formula1>AND(ISDATE(S3), S2&lt;&gt;"")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="M2:M1000">
-      <formula1>AND(ISNUMBER(M2), M2&gt;=0, M2&lt;&gt;"")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="O2:P1000">
-      <formula1>AND(ISTEXT(O2), O2&lt;&gt;" ")</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -21556,82 +21562,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
+    <row r="9">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+    <row r="11">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
+    <row r="13">
+      <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
+    <row r="15">
+      <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
+    <row r="17">
+      <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
+    <row r="19">
+      <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+    <row r="21">
+      <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
+    <row r="23">
+      <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+    <row r="25">
+      <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
+    <row r="27">
+      <c r="A27" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="4" t="s">
+    <row r="29">
+      <c r="A29" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
@@ -21641,27 +21647,27 @@
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>